<commit_message>
Requrest View Insert fix bug delete file fix bug view file
</commit_message>
<xml_diff>
--- a/data dic.xlsx
+++ b/data dic.xlsx
@@ -108,10 +108,10 @@
     <t>RESTATUS</t>
   </si>
   <si>
-    <t>สถานะของคำร้อง (0 = รอดำเนินการ, 1 = อยู่ระหว่างดำเนินการ, 2 = เสร็จสิ้น, 3 = ปฏิเสธ)</t>
-  </si>
-  <si>
     <t>Default: 0</t>
+  </si>
+  <si>
+    <t>สถานะของคำร้อง (0 = รอดำเนินการ, 1 = อยู่ระหว่างดำเนินการ, 2 = เสร็จสิ้น, 3 = ปฏิเสธ, 4 = ถอนคำร้อง)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.09765625" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,10 +604,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>